<commit_message>
fixing confirmation email bug test1
</commit_message>
<xml_diff>
--- a/static/data/ubigeo-peru.xlsx
+++ b/static/data/ubigeo-peru.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20344"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20346"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web_proyects\stickers-gallito-app\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF612359-0B68-485C-A0FF-9C79E7312D50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF9880D-3F97-4A4D-BCA9-DBD94016E339}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ubigeo-peru" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ubigeo-peru'!$A$1:$G$1868</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -5407,7 +5410,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6241,10 +6244,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1868"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -36395,7 +36400,7 @@
         <v>24</v>
       </c>
       <c r="F1311">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G1311">
         <v>8</v>

</xml_diff>